<commit_message>
feat: enhance index page layout and functionality, update API handling for visitas and sendData
</commit_message>
<xml_diff>
--- a/Plantilla VIsitas_TEK.xlsx
+++ b/Plantilla VIsitas_TEK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\za51560\Documents\Programacion\Acceso Diario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E22B997-F6ED-4757-945E-282B9DF28D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F423EEAE-0756-4A6B-A038-D1A22E41DD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15105" yWindow="-16365" windowWidth="29040" windowHeight="15720" xr2:uid="{019328E3-E67A-48E0-8BD1-339FFC7A2A37}"/>
   </bookViews>
@@ -811,7 +811,7 @@
   <dimension ref="B1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:I7"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -887,7 +887,7 @@
         <v>25</v>
       </c>
       <c r="I4" s="14">
-        <v>46007</v>
+        <v>46009</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -913,7 +913,7 @@
         <v>25</v>
       </c>
       <c r="I5" s="14">
-        <v>46007</v>
+        <v>46009</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -937,7 +937,7 @@
         <v>25</v>
       </c>
       <c r="I6" s="14">
-        <v>46007</v>
+        <v>46009</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -961,7 +961,7 @@
         <v>25</v>
       </c>
       <c r="I7" s="14">
-        <v>46007</v>
+        <v>46009</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
feat: update .gitignore to include Excel files and add new Excel templates for visitas
</commit_message>
<xml_diff>
--- a/Plantilla VIsitas_TEK.xlsx
+++ b/Plantilla VIsitas_TEK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\za51560\Documents\Programacion\Acceso Diario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8982CD20-F8B5-47BD-A13A-3D50852042E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E63BDB-3AA8-41D9-965B-D66610E45004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{019328E3-E67A-48E0-8BD1-339FFC7A2A37}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{019328E3-E67A-48E0-8BD1-339FFC7A2A37}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -436,15 +436,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -472,6 +463,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,7 +809,7 @@
   <dimension ref="B1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,40 +825,40 @@
   <sheetData>
     <row r="1" spans="2:10" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="2:10" ht="51" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -872,20 +872,20 @@
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="14">
-        <v>46013</v>
+      <c r="I4" s="11">
+        <v>46017</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -898,20 +898,20 @@
       <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="14">
-        <v>46013</v>
+      <c r="I5" s="11">
+        <v>46017</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -924,18 +924,18 @@
       <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="14">
-        <v>46013</v>
+      <c r="I6" s="11">
+        <v>46017</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -948,89 +948,89 @@
       <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="14">
-        <v>46013</v>
+      <c r="I7" s="11">
+        <v>46017</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="25"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="14"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="11"/>
     </row>
     <row r="9" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="14"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="14"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="11"/>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="17"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="14"/>
     </row>
     <row r="12" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="17"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="14"/>
     </row>
     <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="18"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="15"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="19"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="16"/>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E18" s="2"/>

</xml_diff>